<commit_message>
add 3 rules for  lol
</commit_message>
<xml_diff>
--- a/src/logger.xlsx
+++ b/src/logger.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -2158,28 +2158,378 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>r_one_r1</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
+      <c r="A69" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B69" s="3" t="inlineStr">
         <is>
           <t>2023-12-01</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C69" s="3" t="inlineStr">
         <is>
           <t>14:00:02</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="D69" s="3" t="inlineStr">
         <is>
           <t>code in python a hello world function</t>
         </is>
       </c>
-      <c r="E69" t="n">
+      <c r="E69" s="3" t="n">
         <v>0.00525</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C70" s="3" t="inlineStr">
+        <is>
+          <t>14:40:59</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="inlineStr">
+        <is>
+          <t>Qu'est ce qu'une juridiction en france ?</t>
+        </is>
+      </c>
+      <c r="E70" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B71" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C71" s="3" t="inlineStr">
+        <is>
+          <t>14:43:19</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E71" s="3" t="n">
+        <v>0.00075</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="inlineStr">
+        <is>
+          <t>14:43:31</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="inlineStr">
+        <is>
+          <t>répond moi avec un petit délai</t>
+        </is>
+      </c>
+      <c r="E72" s="3" t="n">
+        <v>0.0045</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B73" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C73" s="3" t="inlineStr">
+        <is>
+          <t>14:43:58</t>
+        </is>
+      </c>
+      <c r="D73" s="3" t="inlineStr">
+        <is>
+          <t>code moi un hellow world en python</t>
+        </is>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B74" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
+        <is>
+          <t>14:44:12</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="inlineStr">
+        <is>
+          <t>code moi un hellow world en python et en c</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>0.0075</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B75" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C75" s="3" t="inlineStr">
+        <is>
+          <t>14:44:41</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="inlineStr">
+        <is>
+          <t>Fais un logo pour unserveur discord epita</t>
+        </is>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B76" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C76" s="3" t="inlineStr">
+        <is>
+          <t>15:04:31</t>
+        </is>
+      </c>
+      <c r="D76" s="3" t="inlineStr">
+        <is>
+          <t>code me in python a hello world function</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B77" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C77" s="3" t="inlineStr">
+        <is>
+          <t>15:04:48</t>
+        </is>
+      </c>
+      <c r="D77" s="3" t="inlineStr">
+        <is>
+          <t>code me in python a hello world function</t>
+        </is>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B78" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="inlineStr">
+        <is>
+          <t>15:06:28</t>
+        </is>
+      </c>
+      <c r="D78" s="3" t="inlineStr">
+        <is>
+          <t>Write me in python, a hello world function</t>
+        </is>
+      </c>
+      <c r="E78" s="3" t="n">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C79" s="3" t="inlineStr">
+        <is>
+          <t>15:06:53</t>
+        </is>
+      </c>
+      <c r="D79" s="3" t="inlineStr">
+        <is>
+          <t>Write me in python, a hello world</t>
+        </is>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B80" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C80" s="3" t="inlineStr">
+        <is>
+          <t>15:07:09</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="inlineStr">
+        <is>
+          <t>Write me in python, a selection sort</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="inlineStr">
+        <is>
+          <t>15:09:42</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="inlineStr">
+        <is>
+          <t>qu'est ce que le circuit d'une loi</t>
+        </is>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>15:11:10</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>ça fait combien 10 minutes par rapport à 2h</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>0.00675</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>15:12:35</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Sur cisco packet tracer, comment répondre à mes questions de TP : 1) ping un ordi 1 via le routeur 2 de l'ip 127.0.0.1</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>0.018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gpt: historic commented and now can handle long requests
</commit_message>
<xml_diff>
--- a/src/logger.xlsx
+++ b/src/logger.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -2708,53 +2708,803 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>r_one_r1</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>2023-12-02</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
+      <c r="A91" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B91" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C91" s="3" t="inlineStr">
         <is>
           <t>18:29:31</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
+      <c r="D91" s="3" t="inlineStr">
         <is>
           <t>dis bonjour</t>
         </is>
       </c>
-      <c r="E91" t="n">
+      <c r="E91" s="3" t="n">
         <v>0.0015</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>r_one_r1</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>2023-12-02</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
+      <c r="A92" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B92" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C92" s="3" t="inlineStr">
         <is>
           <t>18:29:44</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
+      <c r="D92" s="3" t="inlineStr">
         <is>
           <t>qu'ai-je dis avant ?</t>
         </is>
       </c>
-      <c r="E92" t="n">
+      <c r="E92" s="3" t="n">
         <v>0.003</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>18:32:39</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="inlineStr">
+        <is>
+          <t>dis bonjour</t>
+        </is>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>0.0015</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="inlineStr">
+        <is>
+          <t>18:32:49</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="inlineStr">
+        <is>
+          <t>qu'ai-je dis précédemment</t>
+        </is>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>0.00225</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>18:33:49</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="inlineStr">
+        <is>
+          <t>qu'ai je dis avant ?</t>
+        </is>
+      </c>
+      <c r="E95" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="inlineStr">
+        <is>
+          <t>18:34:32</t>
+        </is>
+      </c>
+      <c r="D96" s="3" t="inlineStr">
+        <is>
+          <t>qu'ai je dis avant ?</t>
+        </is>
+      </c>
+      <c r="E96" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
+        <is>
+          <t>18:37:08</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="inlineStr">
+        <is>
+          <t>qu'ai je dis avant ?</t>
+        </is>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="inlineStr">
+        <is>
+          <t>18:37:23</t>
+        </is>
+      </c>
+      <c r="D98" s="3" t="inlineStr">
+        <is>
+          <t>en effet j'avais clear l'histo</t>
+        </is>
+      </c>
+      <c r="E98" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="inlineStr">
+        <is>
+          <t>18:37:37</t>
+        </is>
+      </c>
+      <c r="D99" s="3" t="inlineStr">
+        <is>
+          <t>qu'elle était ma dernière demande</t>
+        </is>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B100" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C100" s="3" t="inlineStr">
+        <is>
+          <t>18:38:16</t>
+        </is>
+      </c>
+      <c r="D100" s="3" t="inlineStr">
+        <is>
+          <t>ai-je dis qqchose avant ?</t>
+        </is>
+      </c>
+      <c r="E100" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B101" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C101" s="3" t="inlineStr">
+        <is>
+          <t>18:39:29</t>
+        </is>
+      </c>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>dernière demande</t>
+        </is>
+      </c>
+      <c r="E101" s="3" t="n">
+        <v>0.0015</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B102" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C102" s="3" t="inlineStr">
+        <is>
+          <t>18:40:03</t>
+        </is>
+      </c>
+      <c r="D102" s="3" t="inlineStr">
+        <is>
+          <t>dernière demande</t>
+        </is>
+      </c>
+      <c r="E102" s="3" t="n">
+        <v>0.0015</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C103" s="3" t="inlineStr">
+        <is>
+          <t>18:40:16</t>
+        </is>
+      </c>
+      <c r="D103" s="3" t="inlineStr">
+        <is>
+          <t>dernière demande</t>
+        </is>
+      </c>
+      <c r="E103" s="3" t="n">
+        <v>0.0015</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="inlineStr">
+        <is>
+          <t>18:40:58</t>
+        </is>
+      </c>
+      <c r="D104" s="3" t="inlineStr">
+        <is>
+          <t>Bonjour</t>
+        </is>
+      </c>
+      <c r="E104" s="3" t="n">
+        <v>0.00075</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="inlineStr">
+        <is>
+          <t>18:41:08</t>
+        </is>
+      </c>
+      <c r="D105" s="3" t="inlineStr">
+        <is>
+          <t>ça va ?</t>
+        </is>
+      </c>
+      <c r="E105" s="3" t="n">
+        <v>0.00225</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B106" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="inlineStr">
+        <is>
+          <t>18:41:40</t>
+        </is>
+      </c>
+      <c r="D106" s="3" t="inlineStr">
+        <is>
+          <t>Qu'ai-je dis avant ?</t>
+        </is>
+      </c>
+      <c r="E106" s="3" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>18:42:05</t>
+        </is>
+      </c>
+      <c r="D107" s="3" t="inlineStr">
+        <is>
+          <t>tu vas bien ?</t>
+        </is>
+      </c>
+      <c r="E107" s="3" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B108" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="inlineStr">
+        <is>
+          <t>18:42:06</t>
+        </is>
+      </c>
+      <c r="D108" s="3" t="inlineStr">
+        <is>
+          <t>tu vas bien ?</t>
+        </is>
+      </c>
+      <c r="E108" s="3" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B109" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C109" s="3" t="inlineStr">
+        <is>
+          <t>18:42:20</t>
+        </is>
+      </c>
+      <c r="D109" s="3" t="inlineStr">
+        <is>
+          <t>pourquoi parfois tu ne réponds pas ?</t>
+        </is>
+      </c>
+      <c r="E109" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B110" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C110" s="3" t="inlineStr">
+        <is>
+          <t>18:42:25</t>
+        </is>
+      </c>
+      <c r="D110" s="3" t="inlineStr">
+        <is>
+          <t>bonjour ?</t>
+        </is>
+      </c>
+      <c r="E110" s="3" t="n">
+        <v>0.0015</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B111" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C111" s="3" t="inlineStr">
+        <is>
+          <t>18:42:35</t>
+        </is>
+      </c>
+      <c r="D111" s="3" t="inlineStr">
+        <is>
+          <t>des fois tu réponds pas</t>
+        </is>
+      </c>
+      <c r="E111" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B112" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C112" s="3" t="inlineStr">
+        <is>
+          <t>18:43:44</t>
+        </is>
+      </c>
+      <c r="D112" s="3" t="inlineStr">
+        <is>
+          <t>bonjouur</t>
+        </is>
+      </c>
+      <c r="E112" s="3" t="n">
+        <v>0.00075</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B113" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C113" s="3" t="inlineStr">
+        <is>
+          <t>18:43:52</t>
+        </is>
+      </c>
+      <c r="D113" s="3" t="inlineStr">
+        <is>
+          <t>ai-je dis quelque chose ?</t>
+        </is>
+      </c>
+      <c r="E113" s="3" t="n">
+        <v>0.00375</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B114" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C114" s="3" t="inlineStr">
+        <is>
+          <t>18:44:09</t>
+        </is>
+      </c>
+      <c r="D114" s="3" t="inlineStr">
+        <is>
+          <t>code me a hello world in python</t>
+        </is>
+      </c>
+      <c r="E114" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B115" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C115" s="3" t="inlineStr">
+        <is>
+          <t>18:44:49</t>
+        </is>
+      </c>
+      <c r="D115" s="3" t="inlineStr">
+        <is>
+          <t>montre moi un petit bout de code</t>
+        </is>
+      </c>
+      <c r="E115" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B116" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C116" s="3" t="inlineStr">
+        <is>
+          <t>18:45:04</t>
+        </is>
+      </c>
+      <c r="D116" s="3" t="inlineStr">
+        <is>
+          <t>montre moi un petit bout de code</t>
+        </is>
+      </c>
+      <c r="E116" s="3" t="n">
+        <v>0.00525</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B117" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C117" s="3" t="inlineStr">
+        <is>
+          <t>18:45:12</t>
+        </is>
+      </c>
+      <c r="D117" s="3" t="inlineStr">
+        <is>
+          <t>bjr</t>
+        </is>
+      </c>
+      <c r="E117" s="3" t="n">
+        <v>0.00075</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B118" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C118" s="3" t="inlineStr">
+        <is>
+          <t>18:46:32</t>
+        </is>
+      </c>
+      <c r="D118" s="3" t="inlineStr">
+        <is>
+          <t>bjr</t>
+        </is>
+      </c>
+      <c r="E118" s="3" t="n">
+        <v>0.00075</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B119" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C119" s="3" t="inlineStr">
+        <is>
+          <t>18:46:53</t>
+        </is>
+      </c>
+      <c r="D119" s="3" t="inlineStr">
+        <is>
+          <t>code me something litle in python</t>
+        </is>
+      </c>
+      <c r="E119" s="3" t="n">
+        <v>0.0045</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B120" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C120" s="3" t="inlineStr">
+        <is>
+          <t>18:47:39</t>
+        </is>
+      </c>
+      <c r="D120" s="3" t="inlineStr">
+        <is>
+          <t>code me something litle in python</t>
+        </is>
+      </c>
+      <c r="E120" s="3" t="n">
+        <v>0.0045</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B121" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C121" s="3" t="inlineStr">
+        <is>
+          <t>18:51:41</t>
+        </is>
+      </c>
+      <c r="D121" s="3" t="inlineStr">
+        <is>
+          <t>code me something litle in python</t>
+        </is>
+      </c>
+      <c r="E121" s="3" t="n">
+        <v>0.0045</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>18:53:03</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>code me heap sort in python</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>0.0045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gpt: change version for gpt4-turbo
</commit_message>
<xml_diff>
--- a/src/logger.xlsx
+++ b/src/logger.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -3483,28 +3483,53 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>r_one_r1</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>2023-12-02</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
+      <c r="A122" s="3" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B122" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C122" s="3" t="inlineStr">
         <is>
           <t>18:53:03</t>
         </is>
       </c>
-      <c r="D122" t="inlineStr">
+      <c r="D122" s="3" t="inlineStr">
         <is>
           <t>code me heap sort in python</t>
         </is>
       </c>
-      <c r="E122" t="n">
+      <c r="E122" s="3" t="n">
         <v>0.0045</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>r_one_r1</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>18:56:13</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>bjr</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>0.00075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>